<commit_message>
actualizacion resumen a mayo 2022
</commit_message>
<xml_diff>
--- a/resumen.xlsx
+++ b/resumen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="-285" windowWidth="8925" windowHeight="7260"/>
+    <workbookView xWindow="570" yWindow="-285" windowWidth="12165" windowHeight="7260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,6 +76,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,11 +108,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P52" sqref="P52"/>
+    <sheetView tabSelected="1" topLeftCell="L10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U40" sqref="U40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3074,7 +3078,7 @@
       <c r="P51">
         <v>500000</v>
       </c>
-      <c r="Q51">
+      <c r="Q51" s="4">
         <v>270341.97027922282</v>
       </c>
       <c r="R51">
@@ -3130,11 +3134,123 @@
       <c r="P52" s="1">
         <v>500000</v>
       </c>
-      <c r="Q52" s="1">
+      <c r="Q52" s="4">
         <v>270761.62</v>
       </c>
       <c r="R52">
         <v>0.54152324802971008</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2022</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>61993</v>
+      </c>
+      <c r="D53" s="1">
+        <v>102908.38</v>
+      </c>
+      <c r="E53" s="1">
+        <v>92.32</v>
+      </c>
+      <c r="F53" s="1">
+        <v>103000.7</v>
+      </c>
+      <c r="G53">
+        <v>42663.24</v>
+      </c>
+      <c r="H53">
+        <v>39531.170000000006</v>
+      </c>
+      <c r="I53">
+        <v>6917.77</v>
+      </c>
+      <c r="J53" s="1">
+        <v>5847.8</v>
+      </c>
+      <c r="K53" s="1">
+        <v>6558</v>
+      </c>
+      <c r="L53">
+        <v>101517.98000000001</v>
+      </c>
+      <c r="M53">
+        <v>1482.7199999999866</v>
+      </c>
+      <c r="N53" s="1">
+        <v>213.03448275861876</v>
+      </c>
+      <c r="O53">
+        <v>2.3917539076992348E-2</v>
+      </c>
+      <c r="P53">
+        <v>500000</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>270974.65849761362</v>
+      </c>
+      <c r="R53">
+        <v>0.54194931699522719</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2022</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <v>61349</v>
+      </c>
+      <c r="D54" s="1">
+        <v>101839.34</v>
+      </c>
+      <c r="E54" s="1">
+        <v>84.99</v>
+      </c>
+      <c r="F54" s="1">
+        <v>101924.33</v>
+      </c>
+      <c r="G54" s="1">
+        <v>38879.949999999997</v>
+      </c>
+      <c r="H54" s="1">
+        <v>40261.050000000003</v>
+      </c>
+      <c r="I54" s="1">
+        <v>7010.62</v>
+      </c>
+      <c r="J54" s="1">
+        <v>3484</v>
+      </c>
+      <c r="K54" s="1">
+        <v>6796</v>
+      </c>
+      <c r="L54" s="1">
+        <v>96431.62</v>
+      </c>
+      <c r="M54" s="1">
+        <v>5492.71</v>
+      </c>
+      <c r="N54" s="1">
+        <v>789.18</v>
+      </c>
+      <c r="O54" s="1">
+        <v>8.9532184713687374E-2</v>
+      </c>
+      <c r="P54" s="1">
+        <v>500000</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>271753.78000000003</v>
+      </c>
+      <c r="R54">
+        <v>0.54350756699522729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion a Julio 2022
</commit_message>
<xml_diff>
--- a/resumen.xlsx
+++ b/resumen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="-285" windowWidth="12165" windowHeight="7260"/>
+    <workbookView xWindow="10710" yWindow="225" windowWidth="9795" windowHeight="7260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,12 +108,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R54"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+    <sheetView tabSelected="1" topLeftCell="N46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P57" sqref="P57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3251,6 +3253,119 @@
       </c>
       <c r="R54">
         <v>0.54350756699522729</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2022</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55">
+        <v>69098</v>
+      </c>
+      <c r="D55" s="5">
+        <f>C55*1.66</f>
+        <v>114702.68</v>
+      </c>
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>114702.68</v>
+      </c>
+      <c r="G55">
+        <v>49382.020000000004</v>
+      </c>
+      <c r="H55">
+        <v>42677.64</v>
+      </c>
+      <c r="I55">
+        <v>7216.52</v>
+      </c>
+      <c r="J55">
+        <v>4709.16</v>
+      </c>
+      <c r="K55">
+        <v>7288</v>
+      </c>
+      <c r="L55">
+        <v>111273.34000000001</v>
+      </c>
+      <c r="M55">
+        <v>3429.339999999982</v>
+      </c>
+      <c r="N55">
+        <v>492.72126436781349</v>
+      </c>
+      <c r="O55">
+        <v>4.963009059596489E-2</v>
+      </c>
+      <c r="P55">
+        <v>500000</v>
+      </c>
+      <c r="Q55">
+        <v>272246.50476198143</v>
+      </c>
+      <c r="R55">
+        <v>0.54449300952396285</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2022</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>88241</v>
+      </c>
+      <c r="D56">
+        <v>146480.06</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>146480.06</v>
+      </c>
+      <c r="G56">
+        <v>56990.159999999996</v>
+      </c>
+      <c r="H56">
+        <v>45450.200000000004</v>
+      </c>
+      <c r="I56">
+        <v>7222.1299999999974</v>
+      </c>
+      <c r="J56">
+        <v>4730.5</v>
+      </c>
+      <c r="K56">
+        <v>10826</v>
+      </c>
+      <c r="L56">
+        <v>125218.98999999999</v>
+      </c>
+      <c r="M56">
+        <v>21261.070000000007</v>
+      </c>
+      <c r="N56">
+        <v>3054.7514367816102</v>
+      </c>
+      <c r="O56">
+        <v>0.24094321233893551</v>
+      </c>
+      <c r="P56">
+        <v>500000</v>
+      </c>
+      <c r="Q56">
+        <v>275066.0550493378</v>
+      </c>
+      <c r="R56">
+        <v>0.55013211009867558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion a Agosto 2022
</commit_message>
<xml_diff>
--- a/resumen.xlsx
+++ b/resumen.xlsx
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P57" sqref="P57"/>
+    <sheetView tabSelected="1" topLeftCell="L43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3366,6 +3366,62 @@
       </c>
       <c r="R56">
         <v>0.55013211009867558</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2022</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>76421</v>
+      </c>
+      <c r="D57" s="1">
+        <v>126858.86</v>
+      </c>
+      <c r="E57" s="1">
+        <v>76.5</v>
+      </c>
+      <c r="F57" s="1">
+        <v>127005.36</v>
+      </c>
+      <c r="G57" s="1">
+        <v>49170.55</v>
+      </c>
+      <c r="H57" s="1">
+        <v>44880.77</v>
+      </c>
+      <c r="I57" s="1">
+        <v>7139</v>
+      </c>
+      <c r="J57" s="1">
+        <v>2385.8000000000002</v>
+      </c>
+      <c r="K57" s="1">
+        <v>8980</v>
+      </c>
+      <c r="L57" s="1">
+        <v>112556.12</v>
+      </c>
+      <c r="M57" s="1">
+        <v>14449.24</v>
+      </c>
+      <c r="N57" s="1">
+        <v>2076.04</v>
+      </c>
+      <c r="O57">
+        <v>0.18907420735138236</v>
+      </c>
+      <c r="P57" s="1">
+        <v>500000</v>
+      </c>
+      <c r="Q57">
+        <v>277166.14269301592</v>
+      </c>
+      <c r="R57">
+        <v>0.55433228538603185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>